<commit_message>
feat(139): discard unused work sheets from workbook
</commit_message>
<xml_diff>
--- a/AccuPay/Resources/schedule-7.1.xlsx
+++ b/AccuPay/Resources/schedule-7.1.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lambert\accupay\AccuPay\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="14355" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -294,7 +297,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###,###,###,##0.00"/>
   </numFmts>
@@ -360,6 +363,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -407,7 +413,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -442,7 +448,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1442,75 +1448,75 @@
         <v>87</v>
       </c>
       <c r="F19" s="6">
-        <f>SUM(F17:F17)</f>
+        <f t="shared" ref="F19:O19" si="0">SUM(F17:F17)</f>
         <v>0</v>
       </c>
       <c r="G19" s="6">
-        <f>SUM(G17:G17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="6">
-        <f>SUM(H17:H17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I19" s="6">
-        <f>SUM(I17:I17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J19" s="6">
-        <f>SUM(J17:J17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K19" s="6">
-        <f>SUM(K17:K17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L19" s="6">
-        <f>SUM(L17:L17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M19" s="6">
-        <f>SUM(M17:M17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N19" s="6">
-        <f>SUM(N17:N17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O19" s="6">
-        <f>SUM(O17:O17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q19" s="6">
-        <f>SUM(Q17:Q17)</f>
+        <f t="shared" ref="Q19:X19" si="1">SUM(Q17:Q17)</f>
         <v>0</v>
       </c>
       <c r="R19" s="6">
-        <f>SUM(R17:R17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S19" s="6">
-        <f>SUM(S17:S17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T19" s="6">
-        <f>SUM(T17:T17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U19" s="6">
-        <f>SUM(U17:U17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V19" s="6">
-        <f>SUM(V17:V17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W19" s="6">
-        <f>SUM(W17:W17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X19" s="6">
-        <f>SUM(X17:X17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1579,28 +1585,4 @@
   <pageMargins left="1.96" right="0.18" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>